<commit_message>
Update CONTROLE DE CAIXA 2024 - 2.xlsx
</commit_message>
<xml_diff>
--- a/CONTROLE DE CAIXA 2024 - 2.xlsx
+++ b/CONTROLE DE CAIXA 2024 - 2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rwick\Desktop\controle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{11BAE797-5678-46DB-8186-ACD2A27C6073}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9366FBC7-ECED-4B1F-B2C6-BAA47829390C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="602" activeTab="3" xr2:uid="{FE6C2AA7-AD1E-4474-8D8C-82FE7A7F47D3}"/>
   </bookViews>
@@ -22,17 +22,28 @@
     <sheet name="VALES" sheetId="4" r:id="rId7"/>
     <sheet name="MATRIZ" sheetId="3" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7812" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7891" uniqueCount="118">
   <si>
     <t>EDIO</t>
   </si>
@@ -374,6 +385,18 @@
   </si>
   <si>
     <t>CDEBITO</t>
+  </si>
+  <si>
+    <t>CORTES</t>
+  </si>
+  <si>
+    <t>3 CORTES</t>
+  </si>
+  <si>
+    <t>PROGRESSIVA</t>
+  </si>
+  <si>
+    <t>PÉ</t>
   </si>
 </sst>
 </file>
@@ -43200,8 +43223,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E04E82EC-6B94-4058-A047-CF4B8AB2810B}">
   <dimension ref="A1:P538"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G92" sqref="G92"/>
+    <sheetView tabSelected="1" topLeftCell="A100" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G110" sqref="F110:G110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -44286,9 +44309,15 @@
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
-      <c r="G39" s="3"/>
+      <c r="E39" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G39" s="3">
+        <v>40</v>
+      </c>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
       <c r="J39" s="2"/>
@@ -44304,7 +44333,7 @@
       <c r="N39" s="2"/>
       <c r="O39" s="3">
         <f t="shared" si="2"/>
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="P39" s="37"/>
     </row>
@@ -44529,7 +44558,7 @@
       </c>
       <c r="G49" s="3">
         <f>SUM(G37:G48)</f>
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="H49" s="4" t="s">
         <v>8</v>
@@ -44556,7 +44585,7 @@
       </c>
       <c r="O49" s="3">
         <f>SUM(O37:O48)</f>
-        <v>330</v>
+        <v>370</v>
       </c>
       <c r="P49" s="37"/>
     </row>
@@ -44580,7 +44609,7 @@
       </c>
       <c r="G50" s="15">
         <f>G49/2</f>
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="H50" s="14" t="s">
         <v>16</v>
@@ -44607,7 +44636,7 @@
       </c>
       <c r="O50" s="15">
         <f>O49/2</f>
-        <v>165</v>
+        <v>185</v>
       </c>
       <c r="P50" s="37"/>
     </row>
@@ -45720,21 +45749,33 @@
       <c r="J88" s="3">
         <v>40</v>
       </c>
-      <c r="K88" s="2"/>
-      <c r="L88" s="2"/>
-      <c r="M88" s="3"/>
+      <c r="K88" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L88" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M88" s="3">
+        <v>160</v>
+      </c>
       <c r="N88" s="2"/>
       <c r="O88" s="3">
         <f>SUM(D88,G88,J88,M88)</f>
-        <v>180</v>
+        <v>340</v>
       </c>
       <c r="P88" s="37"/>
     </row>
     <row r="89" spans="1:16" ht="15.75" thickBot="1">
       <c r="A89" s="48"/>
-      <c r="B89" s="2"/>
-      <c r="C89" s="25"/>
-      <c r="D89" s="2"/>
+      <c r="B89" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C89" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D89" s="2">
+        <v>40</v>
+      </c>
       <c r="E89" s="2" t="s">
         <v>21</v>
       </c>
@@ -45744,24 +45785,42 @@
       <c r="G89" s="3">
         <v>80</v>
       </c>
-      <c r="H89" s="2"/>
-      <c r="I89" s="2"/>
-      <c r="J89" s="2"/>
-      <c r="K89" s="2"/>
-      <c r="L89" s="2"/>
-      <c r="M89" s="3"/>
+      <c r="H89" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I89" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J89" s="2">
+        <v>40</v>
+      </c>
+      <c r="K89" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="L89" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M89" s="3">
+        <v>40</v>
+      </c>
       <c r="N89" s="2"/>
       <c r="O89" s="3">
         <f t="shared" ref="O89:O99" si="5">SUM(D89,G89,J89,M89)</f>
-        <v>80</v>
+        <v>200</v>
       </c>
       <c r="P89" s="37"/>
     </row>
     <row r="90" spans="1:16" ht="14.25" customHeight="1" thickBot="1">
       <c r="A90" s="48"/>
-      <c r="B90" s="2"/>
-      <c r="C90" s="2"/>
-      <c r="D90" s="2"/>
+      <c r="B90" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D90" s="2">
+        <v>35</v>
+      </c>
       <c r="E90" s="2" t="s">
         <v>9</v>
       </c>
@@ -45771,24 +45830,42 @@
       <c r="G90" s="3">
         <v>40</v>
       </c>
-      <c r="H90" s="2"/>
-      <c r="I90" s="2"/>
-      <c r="J90" s="2"/>
-      <c r="K90" s="2"/>
-      <c r="L90" s="2"/>
-      <c r="M90" s="2"/>
+      <c r="H90" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I90" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J90" s="2">
+        <v>75</v>
+      </c>
+      <c r="K90" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L90" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M90" s="2">
+        <v>40</v>
+      </c>
       <c r="N90" s="2"/>
       <c r="O90" s="3">
         <f t="shared" si="5"/>
-        <v>40</v>
+        <v>190</v>
       </c>
       <c r="P90" s="37"/>
     </row>
     <row r="91" spans="1:16" ht="15.75" thickBot="1">
       <c r="A91" s="48"/>
-      <c r="B91" s="2"/>
-      <c r="C91" s="2"/>
-      <c r="D91" s="2"/>
+      <c r="B91" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D91" s="2">
+        <v>40</v>
+      </c>
       <c r="E91" s="2" t="s">
         <v>21</v>
       </c>
@@ -45798,58 +45875,100 @@
       <c r="G91" s="2">
         <v>80</v>
       </c>
-      <c r="H91" s="2"/>
-      <c r="I91" s="2"/>
-      <c r="J91" s="2"/>
+      <c r="H91" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="I91" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J91" s="2">
+        <v>60</v>
+      </c>
       <c r="K91" s="2"/>
       <c r="L91" s="2"/>
       <c r="M91" s="2"/>
       <c r="N91" s="2"/>
       <c r="O91" s="3">
         <f t="shared" si="5"/>
-        <v>80</v>
+        <v>180</v>
       </c>
       <c r="P91" s="37"/>
     </row>
     <row r="92" spans="1:16" ht="15.75" thickBot="1">
       <c r="A92" s="48"/>
-      <c r="B92" s="2"/>
-      <c r="C92" s="2"/>
-      <c r="D92" s="2"/>
-      <c r="E92" s="2"/>
-      <c r="F92" s="2"/>
-      <c r="G92" s="2"/>
-      <c r="H92" s="2"/>
-      <c r="I92" s="2"/>
-      <c r="J92" s="2"/>
+      <c r="B92" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D92" s="2">
+        <v>40</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F92" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G92" s="2">
+        <v>40</v>
+      </c>
+      <c r="H92" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I92" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J92" s="2">
+        <v>40</v>
+      </c>
       <c r="K92" s="2"/>
       <c r="L92" s="2"/>
       <c r="M92" s="2"/>
       <c r="N92" s="2"/>
       <c r="O92" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="P92" s="37"/>
     </row>
     <row r="93" spans="1:16" ht="15.75" thickBot="1">
       <c r="A93" s="48"/>
-      <c r="B93" s="2"/>
-      <c r="C93" s="2"/>
-      <c r="D93" s="2"/>
-      <c r="E93" s="2"/>
-      <c r="F93" s="2"/>
-      <c r="G93" s="2"/>
-      <c r="H93" s="2"/>
-      <c r="I93" s="2"/>
-      <c r="J93" s="2"/>
+      <c r="B93" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D93" s="2">
+        <v>80</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F93" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G93" s="2">
+        <v>35</v>
+      </c>
+      <c r="H93" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I93" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J93" s="2">
+        <v>40</v>
+      </c>
       <c r="K93" s="2"/>
       <c r="L93" s="2"/>
       <c r="M93" s="2"/>
       <c r="N93" s="2"/>
       <c r="O93" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>155</v>
       </c>
       <c r="P93" s="37"/>
     </row>
@@ -45858,9 +45977,15 @@
       <c r="B94" s="2"/>
       <c r="C94" s="2"/>
       <c r="D94" s="2"/>
-      <c r="E94" s="2"/>
-      <c r="F94" s="2"/>
-      <c r="G94" s="2"/>
+      <c r="E94" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G94" s="2">
+        <v>80</v>
+      </c>
       <c r="H94" s="2"/>
       <c r="I94" s="2"/>
       <c r="J94" s="2"/>
@@ -45870,7 +45995,7 @@
       <c r="N94" s="2"/>
       <c r="O94" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="P94" s="37"/>
     </row>
@@ -45879,9 +46004,15 @@
       <c r="B95" s="2"/>
       <c r="C95" s="2"/>
       <c r="D95" s="2"/>
-      <c r="E95" s="2"/>
-      <c r="F95" s="2"/>
-      <c r="G95" s="2"/>
+      <c r="E95" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G95" s="2">
+        <v>40</v>
+      </c>
       <c r="H95" s="2"/>
       <c r="I95" s="2"/>
       <c r="J95" s="2"/>
@@ -45891,7 +46022,7 @@
       <c r="N95" s="2"/>
       <c r="O95" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="P95" s="37"/>
     </row>
@@ -45989,7 +46120,7 @@
       </c>
       <c r="D100" s="3">
         <f>SUM(D88:D99)</f>
-        <v>40</v>
+        <v>275</v>
       </c>
       <c r="E100" s="4" t="s">
         <v>8</v>
@@ -45999,7 +46130,7 @@
       </c>
       <c r="G100" s="3">
         <f>SUM(G88:G99)</f>
-        <v>300</v>
+        <v>495</v>
       </c>
       <c r="H100" s="4" t="s">
         <v>8</v>
@@ -46009,7 +46140,7 @@
       </c>
       <c r="J100" s="3">
         <f>SUM(J88:J99)</f>
-        <v>40</v>
+        <v>295</v>
       </c>
       <c r="K100" s="4" t="s">
         <v>8</v>
@@ -46019,14 +46150,14 @@
       </c>
       <c r="M100" s="3">
         <f>SUM(M88:M99)</f>
-        <v>0</v>
+        <v>240</v>
       </c>
       <c r="N100" s="4" t="s">
         <v>8</v>
       </c>
       <c r="O100" s="3">
         <f>SUM(O88:O99)</f>
-        <v>380</v>
+        <v>1305</v>
       </c>
       <c r="P100" s="37"/>
     </row>
@@ -46040,7 +46171,7 @@
       </c>
       <c r="D101" s="15">
         <f>D100/2</f>
-        <v>20</v>
+        <v>137.5</v>
       </c>
       <c r="E101" s="14" t="s">
         <v>16</v>
@@ -46050,7 +46181,7 @@
       </c>
       <c r="G101" s="15">
         <f>G100/2</f>
-        <v>150</v>
+        <v>247.5</v>
       </c>
       <c r="H101" s="14" t="s">
         <v>16</v>
@@ -46060,7 +46191,7 @@
       </c>
       <c r="J101" s="15">
         <f>J100/2</f>
-        <v>20</v>
+        <v>147.5</v>
       </c>
       <c r="K101" s="14" t="s">
         <v>16</v>
@@ -46070,14 +46201,14 @@
       </c>
       <c r="M101" s="15">
         <f>M100/2</f>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="N101" s="14" t="s">
         <v>16</v>
       </c>
       <c r="O101" s="15">
         <f>O100/2</f>
-        <v>190</v>
+        <v>652.5</v>
       </c>
       <c r="P101" s="37"/>
     </row>
@@ -46173,64 +46304,136 @@
     </row>
     <row r="105" spans="1:16" ht="15.75" thickBot="1">
       <c r="A105" s="48"/>
-      <c r="B105" s="2"/>
-      <c r="C105" s="2"/>
-      <c r="D105" s="3"/>
-      <c r="E105" s="2"/>
-      <c r="F105" s="2"/>
-      <c r="G105" s="3"/>
-      <c r="H105" s="2"/>
-      <c r="I105" s="2"/>
-      <c r="J105" s="3"/>
-      <c r="K105" s="2"/>
-      <c r="L105" s="2"/>
-      <c r="M105" s="3"/>
+      <c r="B105" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D105" s="3">
+        <v>90</v>
+      </c>
+      <c r="E105" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F105" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G105" s="3">
+        <v>35</v>
+      </c>
+      <c r="H105" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I105" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J105" s="3">
+        <v>40</v>
+      </c>
+      <c r="K105" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L105" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M105" s="3">
+        <v>90</v>
+      </c>
       <c r="N105" s="2"/>
       <c r="O105" s="3">
         <f>SUM(D105,G105,J105,M105)</f>
-        <v>0</v>
+        <v>255</v>
       </c>
       <c r="P105" s="37"/>
     </row>
     <row r="106" spans="1:16" ht="15.75" thickBot="1">
       <c r="A106" s="48"/>
-      <c r="B106" s="2"/>
-      <c r="C106" s="2"/>
-      <c r="D106" s="3"/>
-      <c r="E106" s="2"/>
-      <c r="F106" s="2"/>
-      <c r="G106" s="3"/>
-      <c r="H106" s="2"/>
-      <c r="I106" s="2"/>
-      <c r="J106" s="2"/>
-      <c r="K106" s="2"/>
-      <c r="L106" s="2"/>
-      <c r="M106" s="3"/>
+      <c r="B106" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D106" s="3">
+        <v>20</v>
+      </c>
+      <c r="E106" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F106" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G106" s="3">
+        <v>40</v>
+      </c>
+      <c r="H106" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I106" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J106" s="2">
+        <v>40</v>
+      </c>
+      <c r="K106" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L106" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M106" s="3">
+        <v>40</v>
+      </c>
       <c r="N106" s="2"/>
       <c r="O106" s="3">
         <f t="shared" ref="O106:O116" si="6">SUM(D106,G106,J106,M106)</f>
-        <v>0</v>
+        <v>140</v>
       </c>
       <c r="P106" s="37"/>
     </row>
     <row r="107" spans="1:16" ht="15.75" thickBot="1">
       <c r="A107" s="48"/>
-      <c r="B107" s="2"/>
-      <c r="C107" s="2"/>
-      <c r="D107" s="2"/>
-      <c r="E107" s="2"/>
-      <c r="F107" s="2"/>
-      <c r="G107" s="3"/>
-      <c r="H107" s="2"/>
-      <c r="I107" s="2"/>
-      <c r="J107" s="2"/>
-      <c r="K107" s="2"/>
-      <c r="L107" s="2"/>
-      <c r="M107" s="2"/>
+      <c r="B107" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D107" s="2">
+        <v>40</v>
+      </c>
+      <c r="E107" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F107" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G107" s="3">
+        <v>40</v>
+      </c>
+      <c r="H107" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I107" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J107" s="2">
+        <v>40</v>
+      </c>
+      <c r="K107" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L107" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M107" s="2">
+        <v>40</v>
+      </c>
       <c r="N107" s="2"/>
       <c r="O107" s="3">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="P107" s="37"/>
     </row>
@@ -46239,19 +46442,37 @@
       <c r="B108" s="2"/>
       <c r="C108" s="2"/>
       <c r="D108" s="2"/>
-      <c r="E108" s="2"/>
-      <c r="F108" s="2"/>
-      <c r="G108" s="2"/>
-      <c r="H108" s="2"/>
-      <c r="I108" s="2"/>
-      <c r="J108" s="2"/>
-      <c r="K108" s="2"/>
-      <c r="L108" s="2"/>
-      <c r="M108" s="2"/>
+      <c r="E108" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F108" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G108" s="2">
+        <v>40</v>
+      </c>
+      <c r="H108" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I108" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J108" s="2">
+        <v>80</v>
+      </c>
+      <c r="K108" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L108" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M108" s="2">
+        <v>40</v>
+      </c>
       <c r="N108" s="2"/>
       <c r="O108" s="3">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="P108" s="37"/>
     </row>
@@ -46260,19 +46481,37 @@
       <c r="B109" s="2"/>
       <c r="C109" s="2"/>
       <c r="D109" s="2"/>
-      <c r="E109" s="2"/>
-      <c r="F109" s="2"/>
-      <c r="G109" s="2"/>
-      <c r="H109" s="2"/>
-      <c r="I109" s="2"/>
-      <c r="J109" s="2"/>
-      <c r="K109" s="2"/>
-      <c r="L109" s="2"/>
-      <c r="M109" s="2"/>
+      <c r="E109" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F109" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G109" s="2">
+        <v>40</v>
+      </c>
+      <c r="H109" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I109" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J109" s="2">
+        <v>40</v>
+      </c>
+      <c r="K109" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="L109" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M109" s="2">
+        <v>120</v>
+      </c>
       <c r="N109" s="2"/>
       <c r="O109" s="3">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="P109" s="37"/>
     </row>
@@ -46284,16 +46523,28 @@
       <c r="E110" s="2"/>
       <c r="F110" s="2"/>
       <c r="G110" s="2"/>
-      <c r="H110" s="2"/>
-      <c r="I110" s="2"/>
-      <c r="J110" s="2"/>
-      <c r="K110" s="2"/>
-      <c r="L110" s="2"/>
-      <c r="M110" s="2"/>
+      <c r="H110" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I110" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J110" s="2">
+        <v>40</v>
+      </c>
+      <c r="K110" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L110" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M110" s="2">
+        <v>40</v>
+      </c>
       <c r="N110" s="2"/>
       <c r="O110" s="3">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="P110" s="37"/>
     </row>
@@ -46308,13 +46559,19 @@
       <c r="H111" s="2"/>
       <c r="I111" s="2"/>
       <c r="J111" s="2"/>
-      <c r="K111" s="2"/>
-      <c r="L111" s="2"/>
-      <c r="M111" s="2"/>
+      <c r="K111" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L111" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M111" s="2">
+        <v>40</v>
+      </c>
       <c r="N111" s="2"/>
       <c r="O111" s="3">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="P111" s="37"/>
     </row>
@@ -46433,7 +46690,7 @@
       </c>
       <c r="D117" s="3">
         <f>SUM(D105:D116)</f>
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="E117" s="4" t="s">
         <v>8</v>
@@ -46443,7 +46700,7 @@
       </c>
       <c r="G117" s="3">
         <f>SUM(G105:G116)</f>
-        <v>0</v>
+        <v>195</v>
       </c>
       <c r="H117" s="4" t="s">
         <v>8</v>
@@ -46453,7 +46710,7 @@
       </c>
       <c r="J117" s="3">
         <f>SUM(J105:J116)</f>
-        <v>0</v>
+        <v>280</v>
       </c>
       <c r="K117" s="4" t="s">
         <v>8</v>
@@ -46463,14 +46720,14 @@
       </c>
       <c r="M117" s="3">
         <f>SUM(M105:M116)</f>
-        <v>0</v>
+        <v>410</v>
       </c>
       <c r="N117" s="4" t="s">
         <v>8</v>
       </c>
       <c r="O117" s="3">
         <f>SUM(O105:O116)</f>
-        <v>0</v>
+        <v>1035</v>
       </c>
       <c r="P117" s="37"/>
     </row>
@@ -46484,7 +46741,7 @@
       </c>
       <c r="D118" s="15">
         <f>D117/2</f>
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="E118" s="14" t="s">
         <v>16</v>
@@ -46494,7 +46751,7 @@
       </c>
       <c r="G118" s="15">
         <f>G117/2</f>
-        <v>0</v>
+        <v>97.5</v>
       </c>
       <c r="H118" s="14" t="s">
         <v>16</v>
@@ -46504,7 +46761,7 @@
       </c>
       <c r="J118" s="15">
         <f>J117/2</f>
-        <v>0</v>
+        <v>140</v>
       </c>
       <c r="K118" s="14" t="s">
         <v>16</v>
@@ -46514,14 +46771,14 @@
       </c>
       <c r="M118" s="15">
         <f>M117/2</f>
-        <v>0</v>
+        <v>205</v>
       </c>
       <c r="N118" s="14" t="s">
         <v>16</v>
       </c>
       <c r="O118" s="15">
         <f>O117/2</f>
-        <v>0</v>
+        <v>517.5</v>
       </c>
       <c r="P118" s="37"/>
     </row>
@@ -57252,7 +57509,7 @@
       </c>
       <c r="D530" s="38">
         <f>SUM(D15,D32,D49,D66,D83,D100,D117,D134,D151,D168,D185,D202,D219,D236,D253)</f>
-        <v>375</v>
+        <v>760</v>
       </c>
       <c r="E530" s="11" t="s">
         <v>8</v>
@@ -57262,7 +57519,7 @@
       </c>
       <c r="G530" s="38">
         <f>SUM(G15,G32,G49,G66,G83,G100,G117,G134,G151,G168,G185,G202,G219,G236,G253)</f>
-        <v>680</v>
+        <v>1110</v>
       </c>
       <c r="H530" s="11" t="s">
         <v>8</v>
@@ -57272,7 +57529,7 @@
       </c>
       <c r="J530" s="38">
         <f>SUM(J15,J32,J49,J66,J83,J100,J117,J134,J151,J168,J185,J202,J219,J236,J253)</f>
-        <v>355</v>
+        <v>890</v>
       </c>
       <c r="K530" s="11" t="s">
         <v>8</v>
@@ -57282,14 +57539,14 @@
       </c>
       <c r="M530" s="38">
         <f>SUM(M15,M32,M49,M66,M83,M100,M117,M134,M151,M168,M185,M202,M219,M236,M253)</f>
-        <v>355</v>
+        <v>1005</v>
       </c>
       <c r="N530" s="11" t="s">
         <v>8</v>
       </c>
       <c r="O530" s="12">
         <f>SUM(D530,G530,J530,M530)</f>
-        <v>1765</v>
+        <v>3765</v>
       </c>
       <c r="P530" s="37"/>
     </row>
@@ -57303,7 +57560,7 @@
       </c>
       <c r="D531" s="12">
         <f>D530/2</f>
-        <v>187.5</v>
+        <v>380</v>
       </c>
       <c r="E531" s="11" t="s">
         <v>16</v>
@@ -57313,7 +57570,7 @@
       </c>
       <c r="G531" s="12">
         <f>G530/2</f>
-        <v>340</v>
+        <v>555</v>
       </c>
       <c r="H531" s="11" t="s">
         <v>16</v>
@@ -57323,7 +57580,7 @@
       </c>
       <c r="J531" s="12">
         <f>J530/2</f>
-        <v>177.5</v>
+        <v>445</v>
       </c>
       <c r="K531" s="11" t="s">
         <v>16</v>
@@ -57333,14 +57590,14 @@
       </c>
       <c r="M531" s="12">
         <f>M530/2</f>
-        <v>177.5</v>
+        <v>502.5</v>
       </c>
       <c r="N531" s="11" t="s">
         <v>16</v>
       </c>
       <c r="O531" s="12">
         <f>SUM(D531,G531,J531,M531,)</f>
-        <v>882.5</v>
+        <v>1882.5</v>
       </c>
       <c r="P531" s="37"/>
     </row>
@@ -57492,7 +57749,7 @@
       </c>
       <c r="D536" s="38">
         <f>SUM(D530,D533)</f>
-        <v>375</v>
+        <v>760</v>
       </c>
       <c r="E536" s="11" t="s">
         <v>8</v>
@@ -57502,7 +57759,7 @@
       </c>
       <c r="G536" s="38">
         <f>SUM(G530,G533)</f>
-        <v>680</v>
+        <v>1110</v>
       </c>
       <c r="H536" s="11" t="s">
         <v>8</v>
@@ -57512,7 +57769,7 @@
       </c>
       <c r="J536" s="38">
         <f>SUM(J530,J533)</f>
-        <v>355</v>
+        <v>890</v>
       </c>
       <c r="K536" s="11" t="s">
         <v>8</v>
@@ -57522,14 +57779,14 @@
       </c>
       <c r="M536" s="38">
         <f>SUM(M530,M533)</f>
-        <v>355</v>
+        <v>1005</v>
       </c>
       <c r="N536" s="11" t="s">
         <v>8</v>
       </c>
       <c r="O536" s="12">
         <f>SUM(O530,O533)</f>
-        <v>1765</v>
+        <v>3765</v>
       </c>
       <c r="P536" s="37"/>
     </row>
@@ -57543,7 +57800,7 @@
       </c>
       <c r="D537" s="12">
         <f>D536/2</f>
-        <v>187.5</v>
+        <v>380</v>
       </c>
       <c r="E537" s="11" t="s">
         <v>16</v>
@@ -57553,7 +57810,7 @@
       </c>
       <c r="G537" s="12">
         <f>G536/2</f>
-        <v>340</v>
+        <v>555</v>
       </c>
       <c r="H537" s="11" t="s">
         <v>16</v>
@@ -57563,7 +57820,7 @@
       </c>
       <c r="J537" s="12">
         <f>J536/2</f>
-        <v>177.5</v>
+        <v>445</v>
       </c>
       <c r="K537" s="11" t="s">
         <v>16</v>
@@ -57573,14 +57830,14 @@
       </c>
       <c r="M537" s="12">
         <f>M536/2</f>
-        <v>177.5</v>
+        <v>502.5</v>
       </c>
       <c r="N537" s="11" t="s">
         <v>16</v>
       </c>
       <c r="O537" s="12">
         <f>SUM(O531,O534)</f>
-        <v>882.5</v>
+        <v>1882.5</v>
       </c>
       <c r="P537" s="37"/>
     </row>
@@ -57872,7 +58129,7 @@
   <dimension ref="A1:N71"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:C26"/>
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -58441,8 +58698,15 @@
     <row r="28" spans="1:14">
       <c r="A28" s="26"/>
       <c r="C28" s="31"/>
-      <c r="D28" s="26"/>
-      <c r="F28" s="31"/>
+      <c r="D28" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28" s="31">
+        <v>50</v>
+      </c>
       <c r="G28" s="26"/>
       <c r="I28" s="31"/>
       <c r="J28" s="26"/>
@@ -58523,7 +58787,7 @@
       <c r="E35" s="88"/>
       <c r="F35" s="32">
         <f>SUM(F28:F34)</f>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="G35" s="87" t="s">
         <v>8</v>
@@ -58546,7 +58810,7 @@
       </c>
       <c r="N35" s="32">
         <f>SUM(C35,F35,I35,L35)</f>
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="15.75" thickBot="1"/>

</xml_diff>